<commit_message>
Refactor for GoogleSheets and highlight winning team cells
</commit_message>
<xml_diff>
--- a/CFB_Data/CFB Spreadsheet.xlsx
+++ b/CFB_Data/CFB Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/66fc47716e975115/Desktop/CFB_Pickem/CFB_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_B3F99533CDF22796B1291860C7AABD68BCD8B2A2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4741C3DB-AB80-4431-B794-095C89113417}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_B3F99533CDF22796B1291860C7AABD68BCD8B2A2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CB06CAF-CAF5-47F3-AA4E-0E7A5DAC54A8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3924" yWindow="3468" windowWidth="17280" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -3431,6 +3431,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3723,7 +3727,9 @@
   </sheetPr>
   <dimension ref="A1:G865"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>